<commit_message>
Relatively stable release for testing auto-capture and auto-fill features. Will probably be 0.5.20.
</commit_message>
<xml_diff>
--- a/Chrome Extension/Dev/data/LoginElements.xlsx
+++ b/Chrome Extension/Dev/data/LoginElements.xlsx
@@ -10,14 +10,14 @@
     <sheet name="UWallet_e_1346792307963" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UWallet_e_1346792307963!$A$1:$F$316</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UWallet_e_1346792307963!$A$1:$G$316</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="434">
   <si>
     <t>url</t>
   </si>
@@ -1316,6 +1316,9 @@
   </si>
   <si>
     <t>www.airfrance.us/cgi-bin/AF/US/en/common/home/flights/ticket-plane.do</t>
+  </si>
+  <si>
+    <t>num</t>
   </si>
 </sst>
 </file>
@@ -2146,12 +2149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F316"/>
+  <dimension ref="A1:G316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2163,7 +2165,7 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2243,7 +2245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2262,8 +2264,11 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2283,7 +2288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2303,7 +2308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2323,7 +2328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2343,7 +2348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2397,7 +2402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2497,7 +2502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2517,7 +2522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2537,7 +2542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2576,8 +2581,11 @@
       <c r="F21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2617,7 +2625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2637,7 +2645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -2657,7 +2665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2677,7 +2685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2694,7 +2702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2714,7 +2722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -2734,7 +2742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2754,7 +2762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -2894,7 +2902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -2934,7 +2942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -2974,7 +2982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -3014,7 +3022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -3054,7 +3062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -3094,7 +3102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -3114,7 +3122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -3134,7 +3142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -3154,7 +3162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -3174,7 +3182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -3194,7 +3202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -3214,7 +3222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -3234,7 +3242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -3254,7 +3262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -3274,7 +3282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -3294,7 +3302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -3311,7 +3319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -3328,7 +3336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -3348,7 +3356,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>100</v>
       </c>
@@ -3368,7 +3376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>103</v>
       </c>
@@ -3388,7 +3396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -3407,8 +3415,11 @@
       <c r="F63" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -3488,7 +3499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>116</v>
       </c>
@@ -3528,7 +3539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -3562,7 +3573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>122</v>
       </c>
@@ -3602,7 +3613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>126</v>
       </c>
@@ -3642,7 +3653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>127</v>
       </c>
@@ -3682,7 +3693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>130</v>
       </c>
@@ -3722,7 +3733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>132</v>
       </c>
@@ -3742,7 +3753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>132</v>
       </c>
@@ -3761,8 +3772,11 @@
       <c r="F81" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -3782,7 +3796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>136</v>
       </c>
@@ -3802,7 +3816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>137</v>
       </c>
@@ -3822,7 +3836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>137</v>
       </c>
@@ -3842,7 +3856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -3859,7 +3873,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>140</v>
       </c>
@@ -3876,7 +3890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>141</v>
       </c>
@@ -3896,7 +3910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>141</v>
       </c>
@@ -3916,7 +3930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>142</v>
       </c>
@@ -3933,7 +3947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>142</v>
       </c>
@@ -3950,7 +3964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>145</v>
       </c>
@@ -3970,7 +3984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>145</v>
       </c>
@@ -3989,8 +4003,11 @@
       <c r="F93" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G93" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>148</v>
       </c>
@@ -4010,7 +4027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>148</v>
       </c>
@@ -4030,7 +4047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -4070,7 +4087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>154</v>
       </c>
@@ -4110,7 +4127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>155</v>
       </c>
@@ -4150,7 +4167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>156</v>
       </c>
@@ -4187,7 +4204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>158</v>
       </c>
@@ -4221,7 +4238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>159</v>
       </c>
@@ -4255,7 +4272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>160</v>
       </c>
@@ -4295,7 +4312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>163</v>
       </c>
@@ -4335,7 +4352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>165</v>
       </c>
@@ -4375,7 +4392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>167</v>
       </c>
@@ -4435,7 +4452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>171</v>
       </c>
@@ -4475,7 +4492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>176</v>
       </c>
@@ -4515,7 +4532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>179</v>
       </c>
@@ -4549,7 +4566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>181</v>
       </c>
@@ -4589,7 +4606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>186</v>
       </c>
@@ -4629,7 +4646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>189</v>
       </c>
@@ -4666,7 +4683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>192</v>
       </c>
@@ -4700,7 +4717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>193</v>
       </c>
@@ -4740,7 +4757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>194</v>
       </c>
@@ -4780,7 +4797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>197</v>
       </c>
@@ -4820,7 +4837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>199</v>
       </c>
@@ -4860,7 +4877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>204</v>
       </c>
@@ -4900,7 +4917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>207</v>
       </c>
@@ -4960,7 +4977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>213</v>
       </c>
@@ -5000,7 +5017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>216</v>
       </c>
@@ -5034,7 +5051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>219</v>
       </c>
@@ -5074,7 +5091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>222</v>
       </c>
@@ -5114,7 +5131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>223</v>
       </c>
@@ -5154,7 +5171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>227</v>
       </c>
@@ -5214,7 +5231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>233</v>
       </c>
@@ -5254,7 +5271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>234</v>
       </c>
@@ -5294,7 +5311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>239</v>
       </c>
@@ -5334,7 +5351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>244</v>
       </c>
@@ -5374,7 +5391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>247</v>
       </c>
@@ -5414,7 +5431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>248</v>
       </c>
@@ -5454,7 +5471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>253</v>
       </c>
@@ -5494,7 +5511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>256</v>
       </c>
@@ -5534,7 +5551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>259</v>
       </c>
@@ -5574,7 +5591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>260</v>
       </c>
@@ -5614,7 +5631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>263</v>
       </c>
@@ -5654,7 +5671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>268</v>
       </c>
@@ -5694,7 +5711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>269</v>
       </c>
@@ -5734,7 +5751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>274</v>
       </c>
@@ -5768,7 +5785,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>275</v>
       </c>
@@ -5808,7 +5825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>279</v>
       </c>
@@ -5848,7 +5865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>280</v>
       </c>
@@ -5888,7 +5905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>281</v>
       </c>
@@ -5928,7 +5945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>285</v>
       </c>
@@ -5965,7 +5982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>287</v>
       </c>
@@ -6002,7 +6019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>288</v>
       </c>
@@ -6036,7 +6053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>289</v>
       </c>
@@ -6076,7 +6093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>291</v>
       </c>
@@ -6116,7 +6133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>292</v>
       </c>
@@ -6156,7 +6173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>293</v>
       </c>
@@ -6190,7 +6207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>296</v>
       </c>
@@ -6224,7 +6241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>297</v>
       </c>
@@ -6244,7 +6261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>299</v>
       </c>
@@ -6264,7 +6281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>299</v>
       </c>
@@ -6284,7 +6301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>300</v>
       </c>
@@ -6301,7 +6318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>300</v>
       </c>
@@ -6318,7 +6335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>302</v>
       </c>
@@ -6335,7 +6352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>302</v>
       </c>
@@ -6352,7 +6369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>304</v>
       </c>
@@ -6372,7 +6389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>304</v>
       </c>
@@ -6392,7 +6409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>305</v>
       </c>
@@ -6412,7 +6429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>305</v>
       </c>
@@ -6432,7 +6449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>309</v>
       </c>
@@ -6452,7 +6469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>309</v>
       </c>
@@ -6472,7 +6489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>314</v>
       </c>
@@ -6491,8 +6508,11 @@
       <c r="F222" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G222" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>317</v>
       </c>
@@ -6512,7 +6532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>317</v>
       </c>
@@ -6532,7 +6552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>320</v>
       </c>
@@ -6549,7 +6569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>320</v>
       </c>
@@ -6566,7 +6586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>321</v>
       </c>
@@ -6586,7 +6606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>321</v>
       </c>
@@ -6605,8 +6625,11 @@
       <c r="F228" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G228" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>325</v>
       </c>
@@ -6626,7 +6649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>325</v>
       </c>
@@ -6646,7 +6669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>327</v>
       </c>
@@ -6666,7 +6689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>327</v>
       </c>
@@ -6686,7 +6709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>332</v>
       </c>
@@ -6703,7 +6726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>332</v>
       </c>
@@ -6720,7 +6743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>335</v>
       </c>
@@ -6740,7 +6763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>335</v>
       </c>
@@ -6760,7 +6783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>340</v>
       </c>
@@ -6780,7 +6803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>340</v>
       </c>
@@ -6800,7 +6823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>344</v>
       </c>
@@ -6820,7 +6843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>344</v>
       </c>
@@ -6837,7 +6860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>346</v>
       </c>
@@ -6857,7 +6880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>348</v>
       </c>
@@ -6897,7 +6920,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>353</v>
       </c>
@@ -6931,7 +6954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>355</v>
       </c>
@@ -6971,7 +6994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>360</v>
       </c>
@@ -7011,7 +7034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>363</v>
       </c>
@@ -7051,7 +7074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>368</v>
       </c>
@@ -7091,7 +7114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>370</v>
       </c>
@@ -7131,7 +7154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>372</v>
       </c>
@@ -7171,7 +7194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>377</v>
       </c>
@@ -7211,7 +7234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>380</v>
       </c>
@@ -7245,7 +7268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>381</v>
       </c>
@@ -7279,7 +7302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>382</v>
       </c>
@@ -7313,7 +7336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>383</v>
       </c>
@@ -7353,7 +7376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>384</v>
       </c>
@@ -7387,7 +7410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>385</v>
       </c>
@@ -7427,7 +7450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>386</v>
       </c>
@@ -7444,7 +7467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>386</v>
       </c>
@@ -7461,7 +7484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>387</v>
       </c>
@@ -7481,7 +7504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>387</v>
       </c>
@@ -7501,7 +7524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>388</v>
       </c>
@@ -7521,7 +7544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>388</v>
       </c>
@@ -7541,7 +7564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>389</v>
       </c>
@@ -7561,7 +7584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>389</v>
       </c>
@@ -7580,8 +7603,11 @@
       <c r="F279" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G279" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>394</v>
       </c>
@@ -7601,7 +7627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>394</v>
       </c>
@@ -7621,7 +7647,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>395</v>
       </c>
@@ -7641,7 +7667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>395</v>
       </c>
@@ -7661,7 +7687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>396</v>
       </c>
@@ -7681,7 +7707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>396</v>
       </c>
@@ -7701,7 +7727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>398</v>
       </c>
@@ -7721,7 +7747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>398</v>
       </c>
@@ -7741,7 +7767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>399</v>
       </c>
@@ -7781,7 +7807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>400</v>
       </c>
@@ -7821,7 +7847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>401</v>
       </c>
@@ -7858,7 +7884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>405</v>
       </c>
@@ -7892,7 +7918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>408</v>
       </c>
@@ -7932,7 +7958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>413</v>
       </c>
@@ -7972,7 +7998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>415</v>
       </c>
@@ -8012,7 +8038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>419</v>
       </c>
@@ -8052,7 +8078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>422</v>
       </c>
@@ -8072,7 +8098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>422</v>
       </c>
@@ -8092,7 +8118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>425</v>
       </c>
@@ -8112,7 +8138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>425</v>
       </c>
@@ -8132,7 +8158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>428</v>
       </c>
@@ -8152,7 +8178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>428</v>
       </c>
@@ -8171,8 +8197,11 @@
       <c r="F309" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G309" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>429</v>
       </c>
@@ -8192,7 +8221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>429</v>
       </c>
@@ -8211,8 +8240,11 @@
       <c r="F311" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G311" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>430</v>
       </c>
@@ -8229,7 +8261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>431</v>
       </c>
@@ -8249,7 +8281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>431</v>
       </c>
@@ -8269,7 +8301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>432</v>
       </c>
@@ -8289,7 +8321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>432</v>
       </c>
@@ -8308,15 +8340,12 @@
       <c r="F316" t="s">
         <v>15</v>
       </c>
+      <c r="G316" t="s">
+        <v>433</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F316">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="u"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G316"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>